<commit_message>
12 new test cases added
</commit_message>
<xml_diff>
--- a/Software Testing Project - 2017 - Dillon Ward.xlsx
+++ b/Software Testing Project - 2017 - Dillon Ward.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -76,13 +76,299 @@
   </si>
   <si>
     <t>Purpose</t>
+  </si>
+  <si>
+    <t>TC.001</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
+  </si>
+  <si>
+    <t>Open Home While Logged In</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>1. Log In to LinkedIn
+2. Go to Home Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page should bring up feed with people/companies following </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Page brings up feed with people/companies following </t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>TC.002</t>
+  </si>
+  <si>
+    <t>Go to home while logged out</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>1. Log out
+2. Type in the url to home</t>
+  </si>
+  <si>
+    <t>Asks the user to log in</t>
+  </si>
+  <si>
+    <t>The user will be asked to enter their login credentials</t>
+  </si>
+  <si>
+    <t>User is re-directed to /login page</t>
+  </si>
+  <si>
+    <t>TC.003</t>
+  </si>
+  <si>
+    <t>TC.004</t>
+  </si>
+  <si>
+    <t>TC.005</t>
+  </si>
+  <si>
+    <t>TC.006</t>
+  </si>
+  <si>
+    <t>TC.010</t>
+  </si>
+  <si>
+    <t>TC.011</t>
+  </si>
+  <si>
+    <t>TC.012</t>
+  </si>
+  <si>
+    <t>TC.013</t>
+  </si>
+  <si>
+    <t>TC.014</t>
+  </si>
+  <si>
+    <t>TC.015</t>
+  </si>
+  <si>
+    <t>TC.016</t>
+  </si>
+  <si>
+    <t>TC.017</t>
+  </si>
+  <si>
+    <t>TC.018</t>
+  </si>
+  <si>
+    <t>TC.019</t>
+  </si>
+  <si>
+    <t>TC.020</t>
+  </si>
+  <si>
+    <t>Log in without credentials</t>
+  </si>
+  <si>
+    <t>1. Open Login
+2. Do not enter credentials
+3. Press login</t>
+  </si>
+  <si>
+    <t>Error message for credentials</t>
+  </si>
+  <si>
+    <t>An error will be displayed to ask the user to enter their credentials</t>
+  </si>
+  <si>
+    <t>Error bar drops down, asked to enter name and password</t>
+  </si>
+  <si>
+    <t>Login after error redirected to home</t>
+  </si>
+  <si>
+    <t>After the error the user will login and will be sent to the feed</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>Logs in with credentials remembered</t>
+  </si>
+  <si>
+    <t>1. Open Login
+2. Do not enter credentials
+3. Press login
+4. Enter Credentials
+5. Log In</t>
+  </si>
+  <si>
+    <t>Log in with credentials</t>
+  </si>
+  <si>
+    <t>Do not allow login without credentials entered after logging out</t>
+  </si>
+  <si>
+    <t>Open My Network and view my connections</t>
+  </si>
+  <si>
+    <t>1. Open My Network</t>
+  </si>
+  <si>
+    <t>If my Connections are loaded by default</t>
+  </si>
+  <si>
+    <t>After opening my network a view of my connections will be displayed</t>
+  </si>
+  <si>
+    <t>Pending Invitations and People You May Know displays by defailt</t>
+  </si>
+  <si>
+    <t>Open Image from Feed</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on image</t>
+  </si>
+  <si>
+    <t>If image is expanded over the page rather than opens in new window</t>
+  </si>
+  <si>
+    <t>Image expands over the page, not entirely</t>
+  </si>
+  <si>
+    <t>The image will cover the page but not entirely</t>
+  </si>
+  <si>
+    <t>My Connections should open when clicked into My Network, rather than Invites/people I may know</t>
+  </si>
+  <si>
+    <t>Defect No - 0001
+Priority - 1
+Severity - Major</t>
+  </si>
+  <si>
+    <t>TC.007 &amp; TC.008</t>
+  </si>
+  <si>
+    <t>Open Company Page/View Company Jobs</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Open a Company Page from Home
+3. View Jobs from Company with no jobs posted</t>
+  </si>
+  <si>
+    <t>If you can go from the home feed to a company's profile page/if you can view jobs posted by the company but the company should have 0 jobs</t>
+  </si>
+  <si>
+    <t>The Company's Profile Page will load/no jobs posted recently will be displayed</t>
+  </si>
+  <si>
+    <t>The Profile is loaded/no jobs recently posted is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC.009 </t>
+  </si>
+  <si>
+    <t>View Jobs posted by company</t>
+  </si>
+  <si>
+    <t>If Jobs that have been posted by the comapany can be viewed</t>
+  </si>
+  <si>
+    <t>A list of positions should be displayed for that company</t>
+  </si>
+  <si>
+    <t>Jobs for that company are listed</t>
+  </si>
+  <si>
+    <t>Open Article from Home feed</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on an article posted by a company</t>
+  </si>
+  <si>
+    <t>If users are taken away from the home or if the link opens in a new window</t>
+  </si>
+  <si>
+    <t>The user will remain home</t>
+  </si>
+  <si>
+    <t>The user remains home</t>
+  </si>
+  <si>
+    <t>Share Article from Home feed</t>
+  </si>
+  <si>
+    <t>1. Go to home
+2. Open a Company profile page
+3. Open See Jobs</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on Share
+3. Click post</t>
+  </si>
+  <si>
+    <t>If a user can share an article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The article will be shared to the users feed by the user </t>
+  </si>
+  <si>
+    <t>Nothing is shared no errors are thrown</t>
+  </si>
+  <si>
+    <t>Defect No - 0003
+Priority - 2
+Severity - Moderate</t>
+  </si>
+  <si>
+    <t>The sharing functionality works but nothing is shared and the page throws no errors - nothing happens</t>
+  </si>
+  <si>
+    <t>Share Article from Home feed as direct message</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on Share
+3. Click Send as Message
+4. Enter someones name
+5. Click Send</t>
+  </si>
+  <si>
+    <t>If a user can share an article as a direct message</t>
+  </si>
+  <si>
+    <t>The article will be shared to another account</t>
+  </si>
+  <si>
+    <t>Defect No - 0004
+Priority - 3
+Severity - Moderate</t>
+  </si>
+  <si>
+    <t>Nothing happens when articles are shared - sharing does not seem to work at all - nothing happens after sharing</t>
+  </si>
+  <si>
+    <t>Defect No - 0002
+Priority - 4
+Severity - Minor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,8 +398,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,8 +440,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -351,6 +655,17 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -368,73 +683,82 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -723,197 +1047,687 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
+    <col min="11" max="16384" width="22.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="12" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="15" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="18"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="7" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="19" t="s">
+      <c r="F4" s="13"/>
+      <c r="G4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="13"/>
+      <c r="G5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="23"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="24"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" spans="1:15" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" spans="1:15" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="L9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:15" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>14</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>15</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>16</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>17</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>18</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>19</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="E5:F6"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="E4:F4"/>

</xml_diff>

<commit_message>
20 test cases finished
</commit_message>
<xml_diff>
--- a/Software Testing Project - 2017 - Dillon Ward.xlsx
+++ b/Software Testing Project - 2017 - Dillon Ward.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -362,6 +362,155 @@
     <t>Defect No - 0002
 Priority - 4
 Severity - Minor</t>
+  </si>
+  <si>
+    <t>Write an update from Home</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on the text box that says 'Share an Article, photo, or update'
+3. Write something
+4. Click Post</t>
+  </si>
+  <si>
+    <t>If a user can post a status</t>
+  </si>
+  <si>
+    <t>The status will be posted to the feed</t>
+  </si>
+  <si>
+    <t>The status is posted to the feed</t>
+  </si>
+  <si>
+    <t>Send Invite to other user to connect</t>
+  </si>
+  <si>
+    <t>1. Go to My Network
+2. click on connect with someone you are not previously connected with
+3. accept connection
+4. get updates about connection</t>
+  </si>
+  <si>
+    <t>If connections are working on home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connections will work and posts about the person you're ocnnected with will apear on the home page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connections work and updates about the person you're connected with appear on the home page </t>
+  </si>
+  <si>
+    <t>Go to another users profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to My Network
+2. Click on the profile of someone you have already connected with
+</t>
+  </si>
+  <si>
+    <t>Check if other user's profiles load</t>
+  </si>
+  <si>
+    <t>The profile will load</t>
+  </si>
+  <si>
+    <t>The profile of the other user is loaded</t>
+  </si>
+  <si>
+    <t>View Companies in your Network</t>
+  </si>
+  <si>
+    <t>1. Go to Jobs</t>
+  </si>
+  <si>
+    <t>Checks if companies that are relative to your connections are displayed</t>
+  </si>
+  <si>
+    <t>Companies will be displayed along with the people that are connected to the companies</t>
+  </si>
+  <si>
+    <t>Companies are displayed but no the connections who work there</t>
+  </si>
+  <si>
+    <t>Defect No - 0005
+Priority - 5
+Severity - Minor</t>
+  </si>
+  <si>
+    <t>The connections that are related to the companies should display but are not - only the companies</t>
+  </si>
+  <si>
+    <t>Filter Job Preferences to show different jobs</t>
+  </si>
+  <si>
+    <t>1. Go to Jobs
+2. Enter Location
+3. Enter Experience level
+4. Enter Industry
+5. Click Done</t>
+  </si>
+  <si>
+    <t>Check if jobs are filtered based upon preference/location</t>
+  </si>
+  <si>
+    <t>Jobs will be filtered</t>
+  </si>
+  <si>
+    <t>Jobs are filtered</t>
+  </si>
+  <si>
+    <t>Send message through message tab</t>
+  </si>
+  <si>
+    <t>1. Go to Messaging
+2. Send a message to another user</t>
+  </si>
+  <si>
+    <t>Check if a message can be sent to a user via messaging tab</t>
+  </si>
+  <si>
+    <t>Message will be sent and received to another user</t>
+  </si>
+  <si>
+    <t>Message is sent</t>
+  </si>
+  <si>
+    <t>Send message through small messaging window</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Open small messaging window in bottom left corner
+3. Send message to another user</t>
+  </si>
+  <si>
+    <t>Check if small messaging window popup is working</t>
+  </si>
+  <si>
+    <t>Message is sent but not received</t>
+  </si>
+  <si>
+    <t>Defect No - 0006
+Priority - 6
+Severity - Minor</t>
+  </si>
+  <si>
+    <t>The message is being sent on the sender side and can be seen in the chat window but is not received</t>
+  </si>
+  <si>
+    <t>View who has viewed your profile</t>
+  </si>
+  <si>
+    <t>1. Go to Home
+2. Click on Who's viewed your profile</t>
+  </si>
+  <si>
+    <t>See if users who have viewed your profile come up</t>
+  </si>
+  <si>
+    <t>Other user accounts who have viewed your account will come up</t>
+  </si>
+  <si>
+    <t>Other accounts appear</t>
   </si>
 </sst>
 </file>
@@ -683,7 +832,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -706,6 +855,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -754,11 +909,11 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1049,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,7 +1220,9 @@
     <col min="8" max="8" width="25.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="30.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="22.7109375" style="2"/>
+    <col min="11" max="11" width="22.7109375" style="2"/>
+    <col min="12" max="12" width="22.7109375" style="26"/>
+    <col min="13" max="16384" width="22.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1073,14 +1230,14 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
@@ -1090,16 +1247,16 @@
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="27"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
@@ -1109,18 +1266,18 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
+      <c r="L3" s="27"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
@@ -1130,18 +1287,18 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="22" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="L4" s="27"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -1151,18 +1308,18 @@
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="3"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="L5" s="27"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
@@ -1172,14 +1329,14 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="3"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="L6" s="27"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -1189,18 +1346,18 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="11"/>
+      <c r="H7" s="13"/>
       <c r="I7" s="3"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="L7" s="27"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -1217,7 +1374,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="27"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
@@ -1276,16 +1433,16 @@
       <c r="E10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="26" t="s">
         <v>26</v>
       </c>
       <c r="J10" s="7" t="s">
@@ -1308,16 +1465,16 @@
       <c r="E11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="26" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="7" t="s">
@@ -1340,25 +1497,25 @@
       <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="26" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1378,16 +1535,16 @@
       <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="26" t="s">
         <v>54</v>
       </c>
       <c r="J13" s="7" t="s">
@@ -1410,25 +1567,25 @@
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L14" s="26" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1448,19 +1605,19 @@
       <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="J15" s="25" t="s">
+      <c r="J15" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1480,16 +1637,16 @@
       <c r="E16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="26" t="s">
         <v>79</v>
       </c>
       <c r="J16" s="7" t="s">
@@ -1512,16 +1669,16 @@
       <c r="E17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="26" t="s">
         <v>84</v>
       </c>
       <c r="J17" s="7" t="s">
@@ -1544,16 +1701,16 @@
       <c r="E18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="26" t="s">
         <v>89</v>
       </c>
       <c r="J18" s="7" t="s">
@@ -1576,25 +1733,25 @@
       <c r="E19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="26" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1614,29 +1771,29 @@
       <c r="E20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="8" t="s">
         <v>57</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="L20" s="26" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>13</v>
       </c>
@@ -1646,8 +1803,29 @@
       <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>14</v>
       </c>
@@ -1657,8 +1835,29 @@
       <c r="C22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>15</v>
       </c>
@@ -1668,8 +1867,29 @@
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>16</v>
       </c>
@@ -1679,8 +1899,35 @@
       <c r="C24" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>17</v>
       </c>
@@ -1690,8 +1937,29 @@
       <c r="C25" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>18</v>
       </c>
@@ -1701,8 +1969,29 @@
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>19</v>
       </c>
@@ -1712,8 +2001,35 @@
       <c r="C27" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H27" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L27" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>20</v>
       </c>
@@ -1722,6 +2038,27 @@
       </c>
       <c r="C28" s="2" t="s">
         <v>49</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H28" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>